<commit_message>
Bus-Driver - BOM temp spreadsheet
</commit_message>
<xml_diff>
--- a/modules/Bus-Driver/Bus-Driver-BOM.xlsx
+++ b/modules/Bus-Driver/Bus-Driver-BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Bus-Driver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{76BB8B48-6892-4FE1-AACA-12D9D9F47029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EABC2B-6EB2-4E3C-AA1E-1991228D3B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="1485" windowWidth="19665" windowHeight="11385"/>
+    <workbookView xWindow="5280" yWindow="1485" windowWidth="19665" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus-Driver-BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -403,7 +415,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1249,11 +1261,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,12 +1387,9 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
       <c r="E3">
         <f t="shared" ref="E3:E13" si="0">MAX(B3-(C3+D3),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
         <v>29</v>

</xml_diff>